<commit_message>
Add todos os cálculos de mediana, média e moda
</commit_message>
<xml_diff>
--- a/planilhas/Tarefa de estatística 01 - Tabela de Frequencias.xlsx
+++ b/planilhas/Tarefa de estatística 01 - Tabela de Frequencias.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Tabela de frequências</t>
   </si>
@@ -44,78 +44,15 @@
   </si>
   <si>
     <t>moda</t>
-  </si>
-  <si>
-    <t>4.0%</t>
-  </si>
-  <si>
-    <t>8.0%</t>
-  </si>
-  <si>
-    <t>12.0%</t>
-  </si>
-  <si>
-    <t>16.0%</t>
-  </si>
-  <si>
-    <t>20.0%</t>
-  </si>
-  <si>
-    <t>28.000000000000004%</t>
-  </si>
-  <si>
-    <t>32.0%</t>
-  </si>
-  <si>
-    <t>40.0%</t>
-  </si>
-  <si>
-    <t>44.0%</t>
-  </si>
-  <si>
-    <t>48.0%</t>
-  </si>
-  <si>
-    <t>52.0%</t>
-  </si>
-  <si>
-    <t>56.00000000000001%</t>
-  </si>
-  <si>
-    <t>60.0%</t>
-  </si>
-  <si>
-    <t>64.0%</t>
-  </si>
-  <si>
-    <t>68.0%</t>
-  </si>
-  <si>
-    <t>72.0%</t>
-  </si>
-  <si>
-    <t>76.0%</t>
-  </si>
-  <si>
-    <t>84.0%</t>
-  </si>
-  <si>
-    <t>88.0%</t>
-  </si>
-  <si>
-    <t>92.0%</t>
-  </si>
-  <si>
-    <t>96.0%</t>
-  </si>
-  <si>
-    <t>100.0%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="##%"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -153,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,20 +438,23 @@
       <c r="C3">
         <v>0.04</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
+      <c r="D3" s="2">
+        <v>0.04</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
+      <c r="F3" s="2">
+        <v>0.04</v>
       </c>
       <c r="G3">
         <v>56.08</v>
       </c>
       <c r="H3">
         <v>59</v>
+      </c>
+      <c r="I3">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -526,14 +467,17 @@
       <c r="C4">
         <v>0.04</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
+      <c r="D4" s="2">
+        <v>0.04</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
+      <c r="F4" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="I4">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -546,14 +490,17 @@
       <c r="C5">
         <v>0.04</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="D5" s="2">
+        <v>0.04</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>12</v>
+      <c r="F5" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I5">
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -566,14 +513,14 @@
       <c r="C6">
         <v>0.04</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
+      <c r="D6" s="2">
+        <v>0.04</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>13</v>
+      <c r="F6" s="2">
+        <v>0.16</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -586,14 +533,14 @@
       <c r="C7">
         <v>0.04</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
+      <c r="D7" s="2">
+        <v>0.04</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
-        <v>14</v>
+      <c r="F7" s="2">
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -606,14 +553,14 @@
       <c r="C8">
         <v>0.08</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
+      <c r="D8" s="2">
+        <v>0.08</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
+      <c r="F8" s="2">
+        <v>0.28</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -626,14 +573,14 @@
       <c r="C9">
         <v>0.04</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
+      <c r="D9" s="2">
+        <v>0.04</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>16</v>
+      <c r="F9" s="2">
+        <v>0.32</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -646,14 +593,14 @@
       <c r="C10">
         <v>0.08</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
+      <c r="D10" s="2">
+        <v>0.08</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
-      <c r="F10" t="s">
-        <v>17</v>
+      <c r="F10" s="2">
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -666,14 +613,14 @@
       <c r="C11">
         <v>0.04</v>
       </c>
-      <c r="D11" t="s">
-        <v>10</v>
+      <c r="D11" s="2">
+        <v>0.04</v>
       </c>
       <c r="E11">
         <v>11</v>
       </c>
-      <c r="F11" t="s">
-        <v>18</v>
+      <c r="F11" s="2">
+        <v>0.44</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -686,14 +633,14 @@
       <c r="C12">
         <v>0.04</v>
       </c>
-      <c r="D12" t="s">
-        <v>10</v>
+      <c r="D12" s="2">
+        <v>0.04</v>
       </c>
       <c r="E12">
         <v>12</v>
       </c>
-      <c r="F12" t="s">
-        <v>19</v>
+      <c r="F12" s="2">
+        <v>0.48</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -706,14 +653,14 @@
       <c r="C13">
         <v>0.04</v>
       </c>
-      <c r="D13" t="s">
-        <v>10</v>
+      <c r="D13" s="2">
+        <v>0.04</v>
       </c>
       <c r="E13">
         <v>13</v>
       </c>
-      <c r="F13" t="s">
-        <v>20</v>
+      <c r="F13" s="2">
+        <v>0.52</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -726,14 +673,14 @@
       <c r="C14">
         <v>0.04</v>
       </c>
-      <c r="D14" t="s">
-        <v>10</v>
+      <c r="D14" s="2">
+        <v>0.04</v>
       </c>
       <c r="E14">
         <v>14</v>
       </c>
-      <c r="F14" t="s">
-        <v>21</v>
+      <c r="F14" s="2">
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -746,14 +693,14 @@
       <c r="C15">
         <v>0.04</v>
       </c>
-      <c r="D15" t="s">
-        <v>10</v>
+      <c r="D15" s="2">
+        <v>0.04</v>
       </c>
       <c r="E15">
         <v>15</v>
       </c>
-      <c r="F15" t="s">
-        <v>22</v>
+      <c r="F15" s="2">
+        <v>0.6</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -766,14 +713,14 @@
       <c r="C16">
         <v>0.04</v>
       </c>
-      <c r="D16" t="s">
-        <v>10</v>
+      <c r="D16" s="2">
+        <v>0.04</v>
       </c>
       <c r="E16">
         <v>16</v>
       </c>
-      <c r="F16" t="s">
-        <v>23</v>
+      <c r="F16" s="2">
+        <v>0.64</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -786,14 +733,14 @@
       <c r="C17">
         <v>0.04</v>
       </c>
-      <c r="D17" t="s">
-        <v>10</v>
+      <c r="D17" s="2">
+        <v>0.04</v>
       </c>
       <c r="E17">
         <v>17</v>
       </c>
-      <c r="F17" t="s">
-        <v>24</v>
+      <c r="F17" s="2">
+        <v>0.68</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -806,14 +753,14 @@
       <c r="C18">
         <v>0.04</v>
       </c>
-      <c r="D18" t="s">
-        <v>10</v>
+      <c r="D18" s="2">
+        <v>0.04</v>
       </c>
       <c r="E18">
         <v>18</v>
       </c>
-      <c r="F18" t="s">
-        <v>25</v>
+      <c r="F18" s="2">
+        <v>0.72</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -826,14 +773,14 @@
       <c r="C19">
         <v>0.04</v>
       </c>
-      <c r="D19" t="s">
-        <v>10</v>
+      <c r="D19" s="2">
+        <v>0.04</v>
       </c>
       <c r="E19">
         <v>19</v>
       </c>
-      <c r="F19" t="s">
-        <v>26</v>
+      <c r="F19" s="2">
+        <v>0.76</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -846,14 +793,14 @@
       <c r="C20">
         <v>0.08</v>
       </c>
-      <c r="D20" t="s">
-        <v>11</v>
+      <c r="D20" s="2">
+        <v>0.08</v>
       </c>
       <c r="E20">
         <v>21</v>
       </c>
-      <c r="F20" t="s">
-        <v>27</v>
+      <c r="F20" s="2">
+        <v>0.84</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -866,14 +813,14 @@
       <c r="C21">
         <v>0.04</v>
       </c>
-      <c r="D21" t="s">
-        <v>10</v>
+      <c r="D21" s="2">
+        <v>0.04</v>
       </c>
       <c r="E21">
         <v>22</v>
       </c>
-      <c r="F21" t="s">
-        <v>28</v>
+      <c r="F21" s="2">
+        <v>0.88</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -886,14 +833,14 @@
       <c r="C22">
         <v>0.04</v>
       </c>
-      <c r="D22" t="s">
-        <v>10</v>
+      <c r="D22" s="2">
+        <v>0.04</v>
       </c>
       <c r="E22">
         <v>23</v>
       </c>
-      <c r="F22" t="s">
-        <v>29</v>
+      <c r="F22" s="2">
+        <v>0.92</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -906,14 +853,14 @@
       <c r="C23">
         <v>0.04</v>
       </c>
-      <c r="D23" t="s">
-        <v>10</v>
+      <c r="D23" s="2">
+        <v>0.04</v>
       </c>
       <c r="E23">
         <v>24</v>
       </c>
-      <c r="F23" t="s">
-        <v>30</v>
+      <c r="F23" s="2">
+        <v>0.96</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -926,14 +873,14 @@
       <c r="C24">
         <v>0.04</v>
       </c>
-      <c r="D24" t="s">
-        <v>10</v>
+      <c r="D24" s="2">
+        <v>0.04</v>
       </c>
       <c r="E24">
         <v>25</v>
       </c>
-      <c r="F24" t="s">
-        <v>31</v>
+      <c r="F24" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>